<commit_message>
Resultados finales de ejecución y cálculo del chorario
</commit_message>
<xml_diff>
--- a/input/datos_profesores.xlsx
+++ b/input/datos_profesores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MacLeod/Playground/chorario/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED78B526-4B10-BF45-BCBF-B8F4673949EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD12CB4-DFB7-D648-95AF-BEA07569C9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="profesores" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,11 +459,23 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>51837750</v>
+      </c>
+      <c r="C2">
+        <v>51837750</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>52857739</v>
+      </c>
+      <c r="C3">
+        <v>406527</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -505,6 +517,9 @@
       <c r="B7">
         <v>52460550</v>
       </c>
+      <c r="C7">
+        <v>558959</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -524,6 +539,9 @@
       <c r="B9">
         <v>79885769</v>
       </c>
+      <c r="C9">
+        <v>79885769</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -562,11 +580,23 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>1024479509</v>
+      </c>
+      <c r="C13">
+        <v>406593</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>41798596</v>
+      </c>
+      <c r="C14">
+        <v>406544</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -575,6 +605,9 @@
       <c r="B15">
         <v>79403099</v>
       </c>
+      <c r="C15">
+        <v>79403099</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -587,23 +620,29 @@
         <v>406575</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <v>1022362423</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>801363</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>11814968</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>27078</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -611,19 +650,28 @@
         <v>52820679</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>39762772</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>1022336186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1018423989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>